<commit_message>
Added decoupling capacitor and ground testpoints
Added decoupling capacitor and grounded test points to optical transmitter board.

Added "REV 0" to silkscreen of FMC connector board
</commit_message>
<xml_diff>
--- a/MPM/PCB Designs/PCB_BillOfMaterial.xlsx
+++ b/MPM/PCB Designs/PCB_BillOfMaterial.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokument\GitHub\MultiphaseMachines\MPM\PCB Designs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Desktop\EXJOBB\Split boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6F7FEC-50E8-4732-95EB-4B90DFDA49F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B62F32-4435-47FF-A5E7-B13E898CFB07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3B7BB0FD-742C-4D07-AE00-AB24D4F90E43}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Quantity</t>
   </si>
@@ -49,9 +49,6 @@
     <t>SOIC-8</t>
   </si>
   <si>
-    <t>SN75453BD OR-logic Driver</t>
-  </si>
-  <si>
     <t>Part</t>
   </si>
   <si>
@@ -97,7 +94,7 @@
     <t>767-9647</t>
   </si>
   <si>
-    <t>145-5989</t>
+    <t>1206 60 Ohm</t>
   </si>
   <si>
     <t>2.5x2.5mm</t>
@@ -106,9 +103,6 @@
     <t>resistor 0603</t>
   </si>
   <si>
-    <t>https://se.rs-online.com/web/p/peripheral-drivers/1455989/</t>
-  </si>
-  <si>
     <t>300-86-429</t>
   </si>
   <si>
@@ -133,6 +127,9 @@
     <t>302-03-076</t>
   </si>
   <si>
+    <t>100p</t>
+  </si>
+  <si>
     <t>0603 100pF</t>
   </si>
   <si>
@@ -163,19 +160,19 @@
     <t>FMC male</t>
   </si>
   <si>
-    <t>1206 82 Ohm</t>
-  </si>
-  <si>
-    <t>https://www.elfa.se/en/din-rail-power-supply-5v-3a-15w-adjustable-mean-well-mdr-20/p/16976112?q=power+supply+5v&amp;pos=2&amp;origPos=6&amp;origPageSize=50&amp;track=true</t>
-  </si>
-  <si>
-    <t>169-76-112</t>
-  </si>
-  <si>
-    <t>5V, 3A Power supply</t>
-  </si>
-  <si>
-    <t>100pF 0603</t>
+    <t>0603 4.7uF</t>
+  </si>
+  <si>
+    <t>https://www.elfa.se/sv/keramisk-kondensator-7uf-10v-0603-10-epcos-c1608x7s1a475k080ac/p/30198110?q=4.7u&amp;pos=20&amp;origPos=20&amp;origPageSize=50&amp;track=true</t>
+  </si>
+  <si>
+    <t>301-98-110</t>
+  </si>
+  <si>
+    <t>capacitor 0603</t>
+  </si>
+  <si>
+    <t>SN75454BD OR-logic Driver</t>
   </si>
 </sst>
 </file>
@@ -666,7 +663,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +678,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -693,15 +690,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -709,33 +706,28 @@
       <c r="C2">
         <v>18</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>36</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>36</v>
@@ -743,125 +735,127 @@
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5">
         <v>36</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>36</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
         <v>43</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1" xr:uid="{D47BF890-08D7-4B0D-92A2-DA2C8581FEB6}"/>
     <hyperlink ref="D9" r:id="rId2" xr:uid="{59859CE2-4B10-4E26-B024-4E342E9AED31}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{1AEACC59-EDF5-4161-BA76-21A20F40B997}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{4810ED44-CC43-47BC-87CB-248FAFEAF4EA}"/>
-    <hyperlink ref="D5" r:id="rId5" xr:uid="{4903BF7D-6D1D-47D2-8A1B-D8FC7432116B}"/>
-    <hyperlink ref="D3" r:id="rId6" xr:uid="{27D37B7B-0197-4DAF-A1B7-DA046F5A4D7A}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{7AC85EFB-84EE-496B-B6CF-696FEBF63EF8}"/>
-    <hyperlink ref="D11" r:id="rId8" xr:uid="{824BAEF0-06AD-46B8-9440-5C8AD804794A}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{4810ED44-CC43-47BC-87CB-248FAFEAF4EA}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{4903BF7D-6D1D-47D2-8A1B-D8FC7432116B}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{27D37B7B-0197-4DAF-A1B7-DA046F5A4D7A}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{7AC85EFB-84EE-496B-B6CF-696FEBF63EF8}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{EAC7AF2D-2340-45EF-AEEF-00612F261B5F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
-  <drawing r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -885,7 +879,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -897,49 +891,49 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
         <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
         <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -947,7 +941,7 @@
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>2</v>

</xml_diff>

<commit_message>
Mouser links and minimum order added
When Elfa and RS did not have the component, Mouser was added.
The minimum order was added.
</commit_message>
<xml_diff>
--- a/MPM/PCB Designs/PCB_BillOfMaterial.xlsx
+++ b/MPM/PCB Designs/PCB_BillOfMaterial.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Desktop\EXJOBB\Split boards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Testbench_Hardware\PCB_interface_Jonas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B62F32-4435-47FF-A5E7-B13E898CFB07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3B7BB0FD-742C-4D07-AE00-AB24D4F90E43}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="OpticalTransmitterBoard" sheetId="1" r:id="rId1"/>
     <sheet name="FMC Connector board" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Quantity</t>
   </si>
@@ -173,12 +172,39 @@
   </si>
   <si>
     <t>SN75454BD OR-logic Driver</t>
+  </si>
+  <si>
+    <t>https://eu.mouser.com/ProductDetail/Texas-Instruments/SN75454BD?qs=rshUhwi3fbb0CyvT4h26%252BA%3D%3D</t>
+  </si>
+  <si>
+    <t>Mouser part number</t>
+  </si>
+  <si>
+    <t>595-SN75454BD</t>
+  </si>
+  <si>
+    <t>MDR-20-5 - DIN Rail Power Supply, 5V, 3A, 15W, Adjustable</t>
+  </si>
+  <si>
+    <t>https://www.elfa.se/en/din-rail-power-supply-5v-3a-15w-adjustable-mean-well-mdr-20/p/16976112?q=power+supply+5v&amp;pos=2&amp;origPos=6&amp;origPageSize=50&amp;track=true</t>
+  </si>
+  <si>
+    <t>169-76-112</t>
+  </si>
+  <si>
+    <t>Minimum Order</t>
+  </si>
+  <si>
+    <t>https://eu.mouser.com/ProductDetail/Keystone-Electronics/5193TR?qs=vLWxofP3U2xUm2eUxX0VjA%3D%3D</t>
+  </si>
+  <si>
+    <t>534-5193TR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -226,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -234,10 +260,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -257,16 +288,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3252108</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>40821</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>31829</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>14317</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>7539718</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>73051</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>204640</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>46547</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -295,8 +326,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6626679" y="2408464"/>
-          <a:ext cx="7798253" cy="4604230"/>
+          <a:off x="7101864" y="4679082"/>
+          <a:ext cx="7892202" cy="4484961"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -312,14 +343,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>404014</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>503074</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -659,24 +690,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672DE4EB-FF65-4D7C-BE60-F81C7D73F169}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" customWidth="1"/>
-    <col min="4" max="4" width="124.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
-    <col min="6" max="6" width="49.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
+    <col min="7" max="7" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -687,16 +720,22 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -706,9 +745,17 @@
       <c r="C2">
         <v>18</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -718,22 +765,26 @@
       <c r="C3">
         <v>36</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="C4">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -743,14 +794,17 @@
       <c r="C5">
         <v>36</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5">
+        <v>500</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -760,8 +814,17 @@
       <c r="C6">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -771,28 +834,34 @@
       <c r="C7">
         <v>18</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -802,14 +871,17 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -819,14 +891,17 @@
       <c r="C10">
         <v>36</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10">
+        <v>250</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -836,48 +911,72 @@
       <c r="C11">
         <v>36</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" xr:uid="{D47BF890-08D7-4B0D-92A2-DA2C8581FEB6}"/>
-    <hyperlink ref="D9" r:id="rId2" xr:uid="{59859CE2-4B10-4E26-B024-4E342E9AED31}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{4810ED44-CC43-47BC-87CB-248FAFEAF4EA}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{4903BF7D-6D1D-47D2-8A1B-D8FC7432116B}"/>
-    <hyperlink ref="D3" r:id="rId5" xr:uid="{27D37B7B-0197-4DAF-A1B7-DA046F5A4D7A}"/>
-    <hyperlink ref="D10" r:id="rId6" xr:uid="{7AC85EFB-84EE-496B-B6CF-696FEBF63EF8}"/>
-    <hyperlink ref="D11" r:id="rId7" xr:uid="{EAC7AF2D-2340-45EF-AEEF-00612F261B5F}"/>
+    <hyperlink ref="E8" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId2"/>
+    <hyperlink ref="E7" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E3" r:id="rId5"/>
+    <hyperlink ref="E10" r:id="rId6"/>
+    <hyperlink ref="E11" r:id="rId7"/>
+    <hyperlink ref="E12" r:id="rId8"/>
+    <hyperlink ref="E2" r:id="rId9"/>
+    <hyperlink ref="E6" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
-  <drawing r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E220A01-4F64-4A8E-8A1C-1E3B92411809}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="64.42578125" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.44140625" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -888,16 +987,19 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -907,14 +1009,17 @@
       <c r="C2">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -924,14 +1029,17 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -939,7 +1047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -947,16 +1055,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{B73DB611-DEEE-4C93-A4B9-1993C7746C3A}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{3CC15DF6-4194-4C6A-8EB5-B9B8D8947F87}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>

</xml_diff>